<commit_message>
Moving file from RunScore repository to GitHub
</commit_message>
<xml_diff>
--- a/FemaleRoadStd2015.xlsx
+++ b/FemaleRoadStd2015.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan Jones\Documents\AgeGrade\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="4395" windowWidth="18825" windowHeight="7740"/>
+    <workbookView xWindow="-15" yWindow="4395" windowWidth="18825" windowHeight="7740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AgeStdFactors" sheetId="2" r:id="rId1"/>
     <sheet name="AgeStdSec" sheetId="3" r:id="rId2"/>
     <sheet name="AgeStdHMS" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" calcMode="autoNoTable" iterate="1" iterateCount="1" iterateDelta="0"/>
+  <calcPr calcId="171027" calcMode="autoNoTable" iterate="1" iterateCount="1" iterateDelta="0"/>
 </workbook>
 </file>
 
@@ -123,7 +128,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="hh:mm:ss"/>
@@ -140,14 +145,17 @@
       <b/>
       <sz val="18"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -159,6 +167,7 @@
       <b/>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -562,6 +571,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -609,7 +621,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -642,9 +654,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -677,6 +706,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -852,10 +898,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+    <sheetView topLeftCell="A91" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
       <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
@@ -7489,7 +7535,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U100"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
@@ -13964,10 +14010,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U100"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E49" workbookViewId="0">
+      <selection activeCell="K86" sqref="K86"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -18278,7 +18326,9 @@
       <c r="T67" s="13">
         <v>0.72693287037037035</v>
       </c>
-      <c r="U67" s="40"/>
+      <c r="U67" s="40">
+        <v>0.96255787037037033</v>
+      </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
@@ -18341,7 +18391,9 @@
       <c r="T68" s="13">
         <v>0.73865740740740737</v>
       </c>
-      <c r="U68" s="40"/>
+      <c r="U68" s="40">
+        <v>0.97809027777777779</v>
+      </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" s="7">
@@ -18404,7 +18456,9 @@
       <c r="T69" s="13">
         <v>0.75077546296296294</v>
       </c>
-      <c r="U69" s="40"/>
+      <c r="U69" s="40">
+        <v>0.99413194444444442</v>
+      </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70" s="14">
@@ -20178,12 +20232,8 @@
       <c r="N99" s="13">
         <v>0.54140046296296296</v>
       </c>
-      <c r="O99" s="13">
-        <v>1.037962962962963</v>
-      </c>
-      <c r="P99" s="13">
-        <v>1.2545023148148149</v>
-      </c>
+      <c r="O99" s="13"/>
+      <c r="P99" s="13"/>
       <c r="Q99" s="13"/>
       <c r="R99" s="13"/>
       <c r="S99" s="13"/>
@@ -20233,12 +20283,8 @@
       <c r="N100" s="33">
         <v>0.72226851851851848</v>
       </c>
-      <c r="O100" s="33">
-        <v>1.5885069444444444</v>
-      </c>
-      <c r="P100" s="33">
-        <v>1.9198842592592593</v>
-      </c>
+      <c r="O100" s="33"/>
+      <c r="P100" s="33"/>
       <c r="Q100" s="33"/>
       <c r="R100" s="33"/>
       <c r="S100" s="33"/>

</xml_diff>